<commit_message>
Update Solución Taller 4
</commit_message>
<xml_diff>
--- a/2019-1/Taller 4/SolT4P1A.xlsx
+++ b/2019-1/Taller 4/SolT4P1A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablo/GoogleDrive/Work/UdeC/Cursos/2019-1/Optimización/2 Talleres/Taller 4/Enunciado-Solución/Solución/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138E147-9701-0046-897F-B8EFEC1FA627}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F69C23-B5AF-4946-8556-5336A1958799}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problema" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="35">
   <si>
     <t>x1</t>
   </si>
@@ -97,9 +97,6 @@
     <t>x2</t>
   </si>
   <si>
-    <t>x3</t>
-  </si>
-  <si>
     <t>x4</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>f1</t>
   </si>
   <si>
-    <t>f3</t>
-  </si>
-  <si>
     <t>FOA</t>
   </si>
   <si>
@@ -197,6 +191,9 @@
   </si>
   <si>
     <t>Iteraciones.tex</t>
+  </si>
+  <si>
+    <t>x5</t>
   </si>
 </sst>
 </file>
@@ -299,13 +296,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -333,23 +330,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>651933</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>16934</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>118534</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC17566-59D7-6948-9E88-334C68D85813}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8489C409-51D2-5E42-B4DA-B615A2F589F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -365,8 +362,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4461933" y="211667"/>
-          <a:ext cx="2857500" cy="1270000"/>
+          <a:off x="4411133" y="584200"/>
+          <a:ext cx="2679700" cy="1231900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -647,7 +644,7 @@
   <dimension ref="A2:H5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+      <selection activeCell="F2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -660,7 +657,7 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -672,18 +669,18 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -706,7 +703,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -729,7 +726,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>-1</v>
@@ -764,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32927362-6CDC-024F-B63A-BC20E67EFC37}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -782,28 +779,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="K1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+      <c r="B1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="K1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -815,17 +812,17 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,18 +833,18 @@
         <v>2</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -868,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -891,7 +888,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -912,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -935,7 +932,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>-1</v>
@@ -961,10 +958,11 @@
         <v>0</v>
       </c>
       <c r="H5" s="7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K5" s="1">
         <v>-1</v>
@@ -990,7 +988,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -1002,55 +1000,55 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -1070,26 +1068,26 @@
     </row>
     <row r="12" spans="1:17">
       <c r="B12" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="B13" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="B14" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1104,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView zoomScale="189" workbookViewId="0">
-      <selection activeCell="H8" sqref="A4:H8"/>
+      <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1127,44 +1125,44 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="8"/>
-      <c r="K4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
+      <c r="K4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -1176,17 +1174,17 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="9"/>
       <c r="K5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>0</v>
@@ -1198,21 +1196,21 @@
         <v>2</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <f>L6-L$7</f>
@@ -1240,7 +1238,7 @@
       </c>
       <c r="I6" s="10"/>
       <c r="K6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -1267,7 +1265,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1289,9 +1287,9 @@
       </c>
       <c r="I7" s="11"/>
       <c r="K7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="15">
+        <v>14</v>
+      </c>
+      <c r="L7" s="13">
         <v>1</v>
       </c>
       <c r="M7" s="1">
@@ -1316,7 +1314,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>-1</v>
@@ -1343,15 +1341,15 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K8" s="1">
         <v>-1</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="13">
         <v>1</v>
       </c>
       <c r="M8" s="7">
@@ -1367,12 +1365,12 @@
         <v>0</v>
       </c>
       <c r="Q8" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -1384,55 +1382,55 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="5">
         <v>0</v>
@@ -1469,19 +1467,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1499,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1517,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1535,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1553,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1571,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1583,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0C17E1-5248-BE4B-81BC-DE8601155296}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1597,7 +1595,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1610,7 +1608,7 @@
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -1622,19 +1620,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1658,7 +1656,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1681,7 +1679,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>-1</v>
@@ -1702,12 +1700,12 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -1720,7 +1718,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -1732,19 +1730,19 @@
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -1768,7 +1766,7 @@
     <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1791,7 +1789,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>-1</v>
@@ -1812,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>